<commit_message>
added discrete weight calculations
</commit_message>
<xml_diff>
--- a/hardware/drive_calculations/calculations.xlsx
+++ b/hardware/drive_calculations/calculations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>Inputs</t>
   </si>
@@ -23,12 +23,18 @@
     <t>coeff fr.</t>
   </si>
   <si>
-    <t>mass(kg)</t>
+    <t>chassis mass(kg)</t>
   </si>
   <si>
     <t>Bot voltage</t>
   </si>
   <si>
+    <t>Electronics mass (kg)</t>
+  </si>
+  <si>
+    <t>total bot mass (kg)</t>
+  </si>
+  <si>
     <t>Torque (N-m)</t>
   </si>
   <si>
@@ -44,6 +50,9 @@
     <t>no. of wheels</t>
   </si>
   <si>
+    <t>mass (kg)</t>
+  </si>
+  <si>
     <t>wheel info</t>
   </si>
   <si>
@@ -59,6 +68,9 @@
     <t>No.of Motors</t>
   </si>
   <si>
+    <t>mass per motor (kg)</t>
+  </si>
+  <si>
     <t>Stall torque</t>
   </si>
   <si>
@@ -68,6 +80,9 @@
     <t>Top speed (m/s)</t>
   </si>
   <si>
+    <t>Torque Produced</t>
+  </si>
+  <si>
     <t>Motor info (GA12-N20)</t>
   </si>
   <si>
@@ -80,7 +95,7 @@
     <t>Max Cont. Current</t>
   </si>
   <si>
-    <t>Battery info</t>
+    <t>Battery info (2S-LiPo)</t>
   </si>
   <si>
     <t>Current Drawn (A)</t>
@@ -89,7 +104,7 @@
     <t>MCU (ESP-32)</t>
   </si>
   <si>
-    <t>Gyro (MPU-6050)</t>
+    <t>IMU (MPU-6050)</t>
   </si>
   <si>
     <t>Motor Driver (logic)</t>
@@ -104,10 +119,13 @@
     <t>Power Info</t>
   </si>
   <si>
-    <t>desired speed(m/s)</t>
-  </si>
-  <si>
-    <t>desired max acceleration(m/s^2)</t>
+    <t>speed(m/s)</t>
+  </si>
+  <si>
+    <t>max acceleration(m/s^2)</t>
+  </si>
+  <si>
+    <t>desired specs</t>
   </si>
   <si>
     <t>Supply Voltage</t>
@@ -231,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -258,11 +276,18 @@
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
@@ -273,12 +298,6 @@
     <xf borderId="4" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -502,11 +521,12 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="18.63"/>
     <col customWidth="1" min="2" max="2" width="24.88"/>
-    <col customWidth="1" min="3" max="3" width="25.0"/>
-    <col customWidth="1" min="4" max="4" width="26.75"/>
-    <col customWidth="1" min="5" max="6" width="15.88"/>
-    <col customWidth="1" min="7" max="7" width="19.75"/>
-    <col customWidth="1" min="8" max="8" width="13.63"/>
+    <col customWidth="1" min="3" max="4" width="26.75"/>
+    <col customWidth="1" min="5" max="5" width="18.25"/>
+    <col customWidth="1" min="6" max="6" width="17.0"/>
+    <col customWidth="1" min="7" max="7" width="15.88"/>
+    <col customWidth="1" min="8" max="8" width="19.75"/>
+    <col customWidth="1" min="9" max="9" width="13.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -519,9 +539,10 @@
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="4"/>
+      <c r="F1" s="1"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
     </row>
     <row r="2">
       <c r="A2" s="1"/>
@@ -529,9 +550,10 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="4"/>
+      <c r="F2" s="1"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
     </row>
     <row r="3">
       <c r="A3" s="5"/>
@@ -544,56 +566,70 @@
       <c r="D3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="6"/>
+      <c r="E3" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="F3" s="6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="7"/>
+        <v>7</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="7"/>
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" s="8">
         <v>0.8</v>
       </c>
       <c r="C4" s="8">
-        <v>1.5</v>
+        <v>0.04</v>
       </c>
       <c r="D4" s="8">
         <v>12.0</v>
       </c>
-      <c r="E4" s="8"/>
+      <c r="E4" s="8">
+        <v>0.03</v>
+      </c>
       <c r="F4" s="9">
-        <f>C4*C17*(B6/2)*2</f>
-        <v>0.15</v>
-      </c>
-      <c r="G4" s="9">
-        <f>B4*C4*9.81</f>
-        <v>11.772</v>
-      </c>
-      <c r="H4" s="7"/>
+        <f>E8*F8+E10+C4+D6*C6+E4</f>
+        <v>0.35</v>
+      </c>
+      <c r="G4" s="10">
+        <f>F4*C17*(B6/2)*2</f>
+        <v>0.035</v>
+      </c>
+      <c r="H4" s="10">
+        <f>B4*F4*9.81</f>
+        <v>2.7468</v>
+      </c>
+      <c r="I4" s="7"/>
     </row>
     <row r="5">
       <c r="A5" s="6"/>
       <c r="B5" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="7"/>
+        <v>11</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B6" s="8">
         <v>0.1</v>
@@ -601,83 +637,102 @@
       <c r="C6" s="8">
         <v>2.0</v>
       </c>
-      <c r="D6" s="7"/>
+      <c r="D6" s="8">
+        <v>0.03</v>
+      </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
     </row>
     <row r="7">
       <c r="A7" s="6"/>
       <c r="B7" s="6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>17</v>
+        <v>20</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B8" s="8">
-        <v>12.0</v>
+        <v>6.0</v>
       </c>
       <c r="C8" s="8">
         <v>1.0</v>
       </c>
       <c r="D8" s="8">
-        <v>200.0</v>
+        <v>100.0</v>
       </c>
       <c r="E8" s="8">
         <v>2.0</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="G8" s="12">
         <f>16*0.0981</f>
         <v>1.5696</v>
       </c>
-      <c r="G8" s="8">
+      <c r="H8" s="8">
         <v>10.0</v>
       </c>
-      <c r="H8" s="9">
+      <c r="I8" s="10">
         <f>PI()*B6*(D8/60)</f>
-        <v>1.047197551</v>
+        <v>0.5235987756</v>
+      </c>
+      <c r="J8" s="13">
+        <f>G8*H8</f>
+        <v>15.696</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="11"/>
+      <c r="A9" s="14"/>
       <c r="B9" s="6" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="7"/>
+        <v>26</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="7"/>
     </row>
     <row r="10">
       <c r="A10" s="6" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B10" s="8">
         <v>30.0</v>
@@ -685,60 +740,66 @@
       <c r="C10" s="8">
         <v>850.0</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="10">
         <f>B10*(C10/1000)</f>
         <v>25.5</v>
       </c>
-      <c r="E10" s="7"/>
+      <c r="E10" s="8">
+        <v>0.2</v>
+      </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
     </row>
     <row r="11">
-      <c r="A11" s="11"/>
+      <c r="A11" s="14"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="7"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="7"/>
     </row>
     <row r="12">
-      <c r="A12" s="11"/>
-      <c r="B12" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="7"/>
+      <c r="A12" s="14"/>
+      <c r="B12" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="7"/>
     </row>
     <row r="13">
-      <c r="A13" s="15"/>
+      <c r="A13" s="18"/>
       <c r="B13" s="6" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="6" t="s">
-        <v>27</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
       <c r="G13" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H13" s="7"/>
+        <v>32</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" s="7"/>
     </row>
     <row r="14">
       <c r="A14" s="6" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B14" s="8">
         <v>0.15</v>
@@ -746,20 +807,21 @@
       <c r="C14" s="8">
         <v>0.005</v>
       </c>
-      <c r="D14" s="10"/>
+      <c r="D14" s="8"/>
       <c r="E14" s="7"/>
-      <c r="F14" s="16">
+      <c r="F14" s="7"/>
+      <c r="G14" s="9">
         <f>B14+C14+D14+C8*E8</f>
         <v>2.155</v>
       </c>
-      <c r="G14" s="16">
-        <f>C10/F14</f>
+      <c r="H14" s="9">
+        <f>C10/G14</f>
         <v>394.4315545</v>
       </c>
-      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
     </row>
     <row r="15">
-      <c r="A15" s="11"/>
+      <c r="A15" s="14"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="7"/>
@@ -767,23 +829,27 @@
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
     </row>
     <row r="16">
-      <c r="A16" s="11"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="6" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="7"/>
+        <v>36</v>
+      </c>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="7"/>
     </row>
     <row r="17">
-      <c r="A17" s="11"/>
+      <c r="A17" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="B17" s="8">
         <v>1.0</v>
       </c>
@@ -795,6 +861,7 @@
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -815,34 +882,34 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>33</v>
+      <c r="A1" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="17">
+      <c r="A2" s="11">
         <v>3.0</v>
       </c>
-      <c r="B2" s="17">
+      <c r="B2" s="11">
         <v>50.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="17">
+      <c r="A3" s="11">
         <v>6.0</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="11">
         <v>100.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="17">
+      <c r="A4" s="11">
         <v>12.0</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="11">
         <v>200.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
made more torque calculations
</commit_message>
<xml_diff>
--- a/hardware/drive_calculations/calculations.xlsx
+++ b/hardware/drive_calculations/calculations.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Drivetrain_Calc" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="V_RPM" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Motor_Calc" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t>Inputs</t>
   </si>
@@ -35,96 +35,99 @@
     <t>total bot mass (kg)</t>
   </si>
   <si>
+    <t>bot info</t>
+  </si>
+  <si>
+    <t>wheel dia(m)</t>
+  </si>
+  <si>
+    <t>no. of wheels</t>
+  </si>
+  <si>
+    <t>mass (kg)</t>
+  </si>
+  <si>
+    <t>wheel info</t>
+  </si>
+  <si>
+    <t>rated voltage</t>
+  </si>
+  <si>
+    <t>stall current(A) per motor</t>
+  </si>
+  <si>
+    <t>Free RPM @ rated V</t>
+  </si>
+  <si>
+    <t>No.of Motors</t>
+  </si>
+  <si>
+    <t>mass per motor (kg)</t>
+  </si>
+  <si>
+    <t>Stall torque (N-m)</t>
+  </si>
+  <si>
+    <t>Ratio</t>
+  </si>
+  <si>
+    <t>Top speed (m/s)</t>
+  </si>
+  <si>
+    <t>Torque Produced</t>
+  </si>
+  <si>
+    <t>Motor info (GA12-N20)</t>
+  </si>
+  <si>
+    <t>C-rating</t>
+  </si>
+  <si>
+    <t>Capacity (mAh)</t>
+  </si>
+  <si>
+    <t>Max Cont. Current (A)</t>
+  </si>
+  <si>
+    <t>Battery info (2S-LiPo)</t>
+  </si>
+  <si>
+    <t>Current Drawn (A)</t>
+  </si>
+  <si>
+    <t>MCU (ESP-32)</t>
+  </si>
+  <si>
+    <t>IMU (MPU-6050)</t>
+  </si>
+  <si>
+    <t>Motor Driver (logic)</t>
+  </si>
+  <si>
+    <t>Total Current Draw</t>
+  </si>
+  <si>
+    <t>Runtime (h)</t>
+  </si>
+  <si>
+    <t>Runtime (min)</t>
+  </si>
+  <si>
+    <t>Power Info</t>
+  </si>
+  <si>
+    <t>speed(m/s)</t>
+  </si>
+  <si>
+    <t>max acceleration(m/s^2)</t>
+  </si>
+  <si>
     <t>Torque (N-m)</t>
   </si>
   <si>
     <t>Traction Limit Force (N)</t>
   </si>
   <si>
-    <t>bot info</t>
-  </si>
-  <si>
-    <t>wheel dia(m)</t>
-  </si>
-  <si>
-    <t>no. of wheels</t>
-  </si>
-  <si>
-    <t>mass (kg)</t>
-  </si>
-  <si>
-    <t>wheel info</t>
-  </si>
-  <si>
-    <t>rated voltage</t>
-  </si>
-  <si>
-    <t>stall current(A) per motor</t>
-  </si>
-  <si>
-    <t>Free RPM @ rated V</t>
-  </si>
-  <si>
-    <t>No.of Motors</t>
-  </si>
-  <si>
-    <t>mass per motor (kg)</t>
-  </si>
-  <si>
-    <t>Stall torque</t>
-  </si>
-  <si>
-    <t>Ratio</t>
-  </si>
-  <si>
-    <t>Top speed (m/s)</t>
-  </si>
-  <si>
-    <t>Torque Produced</t>
-  </si>
-  <si>
-    <t>Motor info (GA12-N20)</t>
-  </si>
-  <si>
-    <t>C-rating</t>
-  </si>
-  <si>
-    <t>Capacity (mAh)</t>
-  </si>
-  <si>
-    <t>Max Cont. Current</t>
-  </si>
-  <si>
-    <t>Battery info (2S-LiPo)</t>
-  </si>
-  <si>
-    <t>Current Drawn (A)</t>
-  </si>
-  <si>
-    <t>MCU (ESP-32)</t>
-  </si>
-  <si>
-    <t>IMU (MPU-6050)</t>
-  </si>
-  <si>
-    <t>Motor Driver (logic)</t>
-  </si>
-  <si>
-    <t>Total Current Draw</t>
-  </si>
-  <si>
-    <t>Runtime (h)</t>
-  </si>
-  <si>
-    <t>Power Info</t>
-  </si>
-  <si>
-    <t>speed(m/s)</t>
-  </si>
-  <si>
-    <t>max acceleration(m/s^2)</t>
-  </si>
-  <si>
     <t>desired specs</t>
   </si>
   <si>
@@ -132,6 +135,21 @@
   </si>
   <si>
     <t>RPM</t>
+  </si>
+  <si>
+    <t>Rated Torque (kg.cm)</t>
+  </si>
+  <si>
+    <t>Stall Torque (kg.cm)</t>
+  </si>
+  <si>
+    <t>Rated Torque (N-m)</t>
+  </si>
+  <si>
+    <t>Stall Torque (N-m)</t>
+  </si>
+  <si>
+    <t>2s LiPo Battery</t>
   </si>
 </sst>
 </file>
@@ -249,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -278,13 +296,13 @@
     <xf borderId="1" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
@@ -299,6 +317,16 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -520,9 +548,10 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="18.63"/>
-    <col customWidth="1" min="2" max="2" width="24.88"/>
-    <col customWidth="1" min="3" max="4" width="26.75"/>
-    <col customWidth="1" min="5" max="5" width="18.25"/>
+    <col customWidth="1" min="2" max="2" width="15.38"/>
+    <col customWidth="1" min="3" max="3" width="21.13"/>
+    <col customWidth="1" min="4" max="4" width="18.25"/>
+    <col customWidth="1" min="5" max="5" width="19.75"/>
     <col customWidth="1" min="6" max="6" width="17.0"/>
     <col customWidth="1" min="7" max="7" width="15.88"/>
     <col customWidth="1" min="8" max="8" width="19.75"/>
@@ -572,17 +601,13 @@
       <c r="F3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
       <c r="I3" s="7"/>
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="8">
         <v>0.8</v>
@@ -600,26 +625,20 @@
         <f>E8*F8+E10+C4+D6*C6+E4</f>
         <v>0.35</v>
       </c>
-      <c r="G4" s="10">
-        <f>F4*C17*(B6/2)*2</f>
-        <v>0.035</v>
-      </c>
-      <c r="H4" s="10">
-        <f>B4*F4*9.81</f>
-        <v>2.7468</v>
-      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
       <c r="I4" s="7"/>
     </row>
     <row r="5">
       <c r="A5" s="6"/>
       <c r="B5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>10</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>12</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
@@ -629,7 +648,7 @@
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6" s="8">
         <v>0.1</v>
@@ -649,36 +668,36 @@
     <row r="7">
       <c r="A7" s="6"/>
       <c r="B7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="E7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="F7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="G7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="H7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="I7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="J7" s="10" t="s">
         <v>20</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8" s="8">
         <v>6.0</v>
@@ -695,14 +714,14 @@
       <c r="F8" s="8">
         <v>0.01</v>
       </c>
-      <c r="G8" s="12">
-        <f>16*0.0981</f>
+      <c r="G8" s="11">
+        <f>IFS(B8=3, Motor_Calc!G4, B8=6, Motor_Calc!G5, B8=12, Motor_Calc!G6)</f>
         <v>1.5696</v>
       </c>
       <c r="H8" s="8">
         <v>10.0</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="12">
         <f>PI()*B6*(D8/60)</f>
         <v>0.5235987756</v>
       </c>
@@ -714,16 +733,16 @@
     <row r="9">
       <c r="A9" s="14"/>
       <c r="B9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>26</v>
-      </c>
       <c r="E9" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="14"/>
@@ -732,7 +751,7 @@
     </row>
     <row r="10">
       <c r="A10" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B10" s="8">
         <v>30.0</v>
@@ -740,7 +759,7 @@
       <c r="C10" s="8">
         <v>850.0</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="12">
         <f>B10*(C10/1000)</f>
         <v>25.5</v>
       </c>
@@ -766,7 +785,7 @@
     <row r="12">
       <c r="A12" s="14"/>
       <c r="B12" s="15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="17"/>
@@ -779,27 +798,29 @@
     <row r="13">
       <c r="A13" s="18"/>
       <c r="B13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>31</v>
       </c>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
       <c r="G13" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="I13" s="7"/>
     </row>
     <row r="14">
       <c r="A14" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" s="8">
         <v>0.15</v>
@@ -815,10 +836,13 @@
         <v>2.155</v>
       </c>
       <c r="H14" s="9">
-        <f>C10/G14</f>
-        <v>394.4315545</v>
-      </c>
-      <c r="I14" s="7"/>
+        <f>(C10/1000)/G14</f>
+        <v>0.3944315545</v>
+      </c>
+      <c r="I14" s="12">
+        <f>H14*60</f>
+        <v>23.66589327</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="14"/>
@@ -834,13 +858,17 @@
     <row r="16">
       <c r="A16" s="14"/>
       <c r="B16" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="D16" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
+      <c r="E16" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
@@ -848,7 +876,7 @@
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B17" s="8">
         <v>1.0</v>
@@ -856,8 +884,14 @@
       <c r="C17" s="8">
         <v>1.0</v>
       </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
+      <c r="D17" s="12">
+        <f>F4*C17*B6</f>
+        <v>0.035</v>
+      </c>
+      <c r="E17" s="12">
+        <f>B4*F4*9.81</f>
+        <v>2.7468</v>
+      </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
@@ -880,37 +914,129 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="4" max="4" width="18.0"/>
+    <col customWidth="1" min="5" max="5" width="16.88"/>
+    <col customWidth="1" min="6" max="6" width="15.75"/>
+    <col customWidth="1" min="7" max="7" width="14.5"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="11" t="s">
+    <row r="3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="19" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="11">
+      <c r="C3" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1"/>
+      <c r="B4" s="20">
         <v>3.0</v>
       </c>
-      <c r="B2" s="11">
+      <c r="C4" s="20">
         <v>50.0</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="11">
+      <c r="D4" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="F4" s="4">
+        <f t="shared" ref="F4:G4" si="1">0.0981*D4</f>
+        <v>0.0981</v>
+      </c>
+      <c r="G4" s="4">
+        <f t="shared" si="1"/>
+        <v>0.7848</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1"/>
+      <c r="B5" s="20">
         <v>6.0</v>
       </c>
-      <c r="B3" s="11">
+      <c r="C5" s="20">
         <v>100.0</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="11">
+      <c r="D5" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>16.0</v>
+      </c>
+      <c r="F5" s="4">
+        <f t="shared" ref="F5:G5" si="2">0.0981*D5</f>
+        <v>0.1962</v>
+      </c>
+      <c r="G5" s="4">
+        <f t="shared" si="2"/>
+        <v>1.5696</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1"/>
+      <c r="B6" s="20">
         <v>12.0</v>
       </c>
-      <c r="B4" s="11">
+      <c r="C6" s="20">
         <v>200.0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>32.0</v>
+      </c>
+      <c r="F6" s="4">
+        <f t="shared" ref="F6:G6" si="3">0.0981*D6</f>
+        <v>0.3924</v>
+      </c>
+      <c r="G6" s="4">
+        <f t="shared" si="3"/>
+        <v>3.1392</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="21">
+        <v>7.4</v>
+      </c>
+      <c r="C7" s="22">
+        <f>B7/B5 * C5</f>
+        <v>123.3333333</v>
+      </c>
+      <c r="D7" s="22">
+        <f>(B7/B5)*D5</f>
+        <v>2.466666667</v>
+      </c>
+      <c r="E7" s="22">
+        <f>B7/B5 * E5</f>
+        <v>19.73333333</v>
+      </c>
+      <c r="F7" s="22">
+        <f t="shared" ref="F7:G7" si="4">0.0981*D7</f>
+        <v>0.24198</v>
+      </c>
+      <c r="G7" s="22">
+        <f t="shared" si="4"/>
+        <v>1.93584</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added rated torque in main table
</commit_message>
<xml_diff>
--- a/hardware/drive_calculations/calculations.xlsx
+++ b/hardware/drive_calculations/calculations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>Inputs</t>
   </si>
@@ -65,6 +65,9 @@
     <t>mass per motor (kg)</t>
   </si>
   <si>
+    <t>Rated Torque(N-m)</t>
+  </si>
+  <si>
     <t>Stall torque (N-m)</t>
   </si>
   <si>
@@ -74,9 +77,6 @@
     <t>Top speed (m/s)</t>
   </si>
   <si>
-    <t>Torque Produced</t>
-  </si>
-  <si>
     <t>Motor info (GA12-N20)</t>
   </si>
   <si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>Max Cont. Current (A)</t>
+  </si>
+  <si>
+    <t>Nominal Voltage (V)</t>
   </si>
   <si>
     <t>Battery info (2S-LiPo)</t>
@@ -267,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -296,16 +299,12 @@
     <xf borderId="1" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
@@ -553,9 +552,9 @@
     <col customWidth="1" min="4" max="4" width="18.25"/>
     <col customWidth="1" min="5" max="5" width="19.75"/>
     <col customWidth="1" min="6" max="6" width="17.0"/>
-    <col customWidth="1" min="7" max="7" width="15.88"/>
-    <col customWidth="1" min="8" max="8" width="19.75"/>
-    <col customWidth="1" min="9" max="9" width="13.63"/>
+    <col customWidth="1" min="7" max="8" width="15.88"/>
+    <col customWidth="1" min="9" max="9" width="19.75"/>
+    <col customWidth="1" min="10" max="10" width="13.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -572,6 +571,7 @@
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
     </row>
     <row r="2">
       <c r="A2" s="1"/>
@@ -583,6 +583,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
     </row>
     <row r="3">
       <c r="A3" s="5"/>
@@ -603,7 +604,8 @@
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="7"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="7"/>
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
@@ -628,6 +630,7 @@
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
     </row>
     <row r="5">
       <c r="A5" s="6"/>
@@ -645,6 +648,7 @@
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
@@ -664,6 +668,7 @@
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
     </row>
     <row r="7">
       <c r="A7" s="6"/>
@@ -691,7 +696,7 @@
       <c r="I7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="6" t="s">
         <v>20</v>
       </c>
     </row>
@@ -714,24 +719,24 @@
       <c r="F8" s="8">
         <v>0.01</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="10">
+        <f>IFS(B8=3, Motor_Calc!F4, B8=6, Motor_Calc!F5, B8=12, Motor_Calc!F6)</f>
+        <v>0.1962</v>
+      </c>
+      <c r="H8" s="10">
         <f>IFS(B8=3, Motor_Calc!G4, B8=6, Motor_Calc!G5, B8=12, Motor_Calc!G6)</f>
         <v>1.5696</v>
       </c>
-      <c r="H8" s="8">
+      <c r="I8" s="8">
         <v>10.0</v>
       </c>
-      <c r="I8" s="12">
+      <c r="J8" s="11">
         <f>PI()*B6*(D8/60)</f>
         <v>0.5235987756</v>
       </c>
-      <c r="J8" s="13">
-        <f>G8*H8</f>
-        <v>15.696</v>
-      </c>
     </row>
     <row r="9">
-      <c r="A9" s="14"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="6" t="s">
         <v>22</v>
       </c>
@@ -744,14 +749,17 @@
       <c r="E9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="7"/>
+      <c r="F9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="7"/>
     </row>
     <row r="10">
       <c r="A10" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" s="8">
         <v>30.0</v>
@@ -759,68 +767,74 @@
       <c r="C10" s="8">
         <v>850.0</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="11">
         <f>B10*(C10/1000)</f>
         <v>25.5</v>
       </c>
       <c r="E10" s="8">
         <v>0.2</v>
       </c>
-      <c r="F10" s="7"/>
+      <c r="F10" s="8">
+        <v>7.4</v>
+      </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
     </row>
     <row r="11">
-      <c r="A11" s="14"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="7"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="7"/>
     </row>
     <row r="12">
-      <c r="A12" s="14"/>
-      <c r="B12" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="7"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="7"/>
     </row>
     <row r="13">
-      <c r="A13" s="18"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="6" t="s">
         <v>30</v>
       </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="6"/>
       <c r="H13" s="6" t="s">
         <v>31</v>
       </c>
       <c r="I13" s="6" t="s">
         <v>32</v>
       </c>
+      <c r="J13" s="6" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B14" s="8">
         <v>0.15</v>
@@ -831,21 +845,22 @@
       <c r="D14" s="8"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
-      <c r="G14" s="9">
+      <c r="G14" s="5"/>
+      <c r="H14" s="9">
         <f>B14+C14+D14+C8*E8</f>
         <v>2.155</v>
       </c>
-      <c r="H14" s="9">
-        <f>(C10/1000)/G14</f>
+      <c r="I14" s="9">
+        <f>(C10/1000)/H14</f>
         <v>0.3944315545</v>
       </c>
-      <c r="I14" s="12">
-        <f>H14*60</f>
+      <c r="J14" s="11">
+        <f>I14*60</f>
         <v>23.66589327</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="14"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="7"/>
@@ -854,29 +869,31 @@
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
     </row>
     <row r="16">
-      <c r="A16" s="14"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="7"/>
+        <v>38</v>
+      </c>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="7"/>
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B17" s="8">
         <v>1.0</v>
@@ -884,11 +901,11 @@
       <c r="C17" s="8">
         <v>1.0</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="11">
         <f>F4*C17*B6</f>
         <v>0.035</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="11">
         <f>B4*F4*9.81</f>
         <v>2.7468</v>
       </c>
@@ -896,6 +913,7 @@
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -923,31 +941,31 @@
   <sheetData>
     <row r="3">
       <c r="A3" s="1"/>
-      <c r="B3" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="19" t="s">
+      <c r="B3" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="C3" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="D3" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="E3" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="F3" s="17" t="s">
         <v>44</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1"/>
-      <c r="B4" s="20">
+      <c r="B4" s="18">
         <v>3.0</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="18">
         <v>50.0</v>
       </c>
       <c r="D4" s="1">
@@ -967,10 +985,10 @@
     </row>
     <row r="5">
       <c r="A5" s="1"/>
-      <c r="B5" s="20">
+      <c r="B5" s="18">
         <v>6.0</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="18">
         <v>100.0</v>
       </c>
       <c r="D5" s="1">
@@ -990,10 +1008,10 @@
     </row>
     <row r="6">
       <c r="A6" s="1"/>
-      <c r="B6" s="20">
+      <c r="B6" s="18">
         <v>12.0</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C6" s="18">
         <v>200.0</v>
       </c>
       <c r="D6" s="1">
@@ -1012,29 +1030,29 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" s="21">
+      <c r="A7" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="19">
         <v>7.4</v>
       </c>
-      <c r="C7" s="22">
+      <c r="C7" s="20">
         <f>B7/B5 * C5</f>
         <v>123.3333333</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="20">
         <f>(B7/B5)*D5</f>
         <v>2.466666667</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="20">
         <f>B7/B5 * E5</f>
         <v>19.73333333</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="20">
         <f t="shared" ref="F7:G7" si="4">0.0981*D7</f>
         <v>0.24198</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G7" s="20">
         <f t="shared" si="4"/>
         <v>1.93584</v>
       </c>

</xml_diff>